<commit_message>
CPT-280 style: customize header row's stylings
</commit_message>
<xml_diff>
--- a/packages/i18n/excels/common.xlsx
+++ b/packages/i18n/excels/common.xlsx
@@ -16,17 +16,17 @@
     <t>Lang Key</t>
   </si>
   <si>
-    <t>zh</t>
+    <t>Locale: zh</t>
   </si>
   <si>
-    <t>en</t>
+    <t>Locale: en</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -35,7 +35,13 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
+      <color rgb="000000"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="3d3fea"/>
       <sz val="12"/>
       <name val="Calibri"/>
     </font>
@@ -60,10 +66,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,23 +419,24 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="3" width="50" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50" style="1" customWidth="1"/>
+    <col min="2" max="3" width="150" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="40" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CPT-280 feat: hightlight rows if any translation is missing
</commit_message>
<xml_diff>
--- a/packages/i18n/excels/common.xlsx
+++ b/packages/i18n/excels/common.xlsx
@@ -11,15 +11,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Lang Key</t>
   </si>
   <si>
-    <t>Locale: zh</t>
-  </si>
-  <si>
-    <t>Locale: en</t>
+    <t>zh</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>/head/description</t>
+  </si>
+  <si>
+    <t>测试</t>
+  </si>
+  <si>
+    <t>Welcome to the TiDB community! Here you can get involved &amp; contribute to the best open source, open-source, cloud-native, distributed SQL database for elastic scale and real-time analytics.</t>
+  </si>
+  <si>
+    <t>/head/titleSuffix</t>
+  </si>
+  <si>
+    <t>TiDB Community</t>
   </si>
 </sst>
 </file>
@@ -35,23 +50,28 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <color rgb="000000"/>
+      <color rgb="ff000000"/>
       <sz val="12"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <color rgb="3d3fea"/>
+      <color rgb="ff3d3fea"/>
       <sz val="12"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ffffff00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,7 +86,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -76,6 +96,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -416,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -426,7 +450,7 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="50" style="1" customWidth="1"/>
-    <col min="2" max="3" width="150" style="1" customWidth="1"/>
+    <col min="2" max="3" width="100" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="40" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -438,6 +462,26 @@
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>